<commit_message>
Minor edits to Excel file
</commit_message>
<xml_diff>
--- a/vm-spinal-risk/output/risk_survey_analysis_jm.xlsx
+++ b/vm-spinal-risk/output/risk_survey_analysis_jm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnmichael/Documents/vm-spinal-risk/vm-spinal-risk/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF73C8AB-7D6C-394E-964C-02FB0C03F544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD1458F-2C2A-1A46-9C49-DE4E4EF4EEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30080" yWindow="500" windowWidth="30080" windowHeight="33340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14766,7 +14766,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated Excel file with removed questions
</commit_message>
<xml_diff>
--- a/vm-spinal-risk/output/risk_survey_analysis_jm.xlsx
+++ b/vm-spinal-risk/output/risk_survey_analysis_jm.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnmichael/Documents/vm-spinal-risk/vm-spinal-risk/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB05C5F1-DE1E-F340-B467-E4D35DDA4B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9177FB-F013-E64A-A29D-EBF697674344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Risk Questions Correlation" sheetId="6" r:id="rId1"/>
-    <sheet name="Risk Questions Distribution" sheetId="4" r:id="rId2"/>
-    <sheet name="Survey Data -&gt;" sheetId="2" r:id="rId3"/>
-    <sheet name="RiskTrial2_DATA_2024-01-18_2039" sheetId="1" r:id="rId4"/>
+    <sheet name="Final Survey" sheetId="7" r:id="rId2"/>
+    <sheet name="Risk Questions Distribution" sheetId="4" r:id="rId3"/>
+    <sheet name="Survey Data -&gt;" sheetId="2" r:id="rId4"/>
+    <sheet name="RiskTrial2_DATA_2024-01-18_2039" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Risk Questions Correlation'!$A$2:$E$782</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'RiskTrial2_DATA_2024-01-18_2039'!$A$1:$BB$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'RiskTrial2_DATA_2024-01-18_2039'!$A$1:$BB$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="195">
   <si>
     <t>record_id</t>
   </si>
@@ -574,6 +575,57 @@
   </si>
   <si>
     <t>Risk Question 2 Survey Number</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t># Questions</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
+  <si>
+    <t>Dospert</t>
+  </si>
+  <si>
+    <t>Attn Check</t>
+  </si>
+  <si>
+    <t>Demographics</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>ODI</t>
+  </si>
+  <si>
+    <t>plus surgery question</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Pain</t>
+  </si>
+  <si>
+    <t>Equal buckets</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Behavior, risk</t>
+  </si>
+  <si>
+    <t>Behavior, spinal risk</t>
   </si>
 </sst>
 </file>
@@ -1587,9 +1639,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9292B732-C7B7-324C-BF47-767C1D07021E}">
   <dimension ref="A1:E782"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14887,14 +14939,138 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473A77DC-DEE7-FA4E-A4DA-0B040495C57E}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="6">
+        <f>SUM(B2:B6)</f>
+        <v>92</v>
+      </c>
+      <c r="C7" s="6">
+        <f>SUM(C2:C6)</f>
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6D9FD0-74D1-024E-ABE3-F746E7332A16}">
   <dimension ref="A1:AP39"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL3" sqref="AL3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14910,6 +15086,60 @@
       <c r="B1" s="6">
         <f>COUNTIFS('RiskTrial2_DATA_2024-01-18_2039'!$BB:$BB,2)</f>
         <v>81</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="AM1" s="6"/>
+      <c r="AN1" s="6"/>
+      <c r="AO1" s="6"/>
+      <c r="AP1" s="6" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:42" ht="34" x14ac:dyDescent="0.2">
@@ -16635,1021 +16865,1021 @@
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>A4</f>
+        <f t="shared" ref="A15:B20" si="2">A4</f>
         <v>Not at All</v>
       </c>
       <c r="B15">
-        <f>B4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C15" s="17">
-        <f>C4/$B$1</f>
+        <f t="shared" ref="C15:AP15" si="3">C4/$B$1</f>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="D15" s="17">
-        <f>D4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="E15" s="17">
-        <f>E4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.43209876543209874</v>
       </c>
       <c r="F15" s="46">
-        <f>F4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.7407407407407407</v>
       </c>
       <c r="G15" s="17">
-        <f>G4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="H15" s="17">
-        <f>H4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>6.1728395061728392E-2</v>
       </c>
       <c r="I15" s="17">
-        <f>I4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.23456790123456789</v>
       </c>
       <c r="J15" s="46">
-        <f>J4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.62962962962962965</v>
       </c>
       <c r="K15" s="22">
-        <f>K4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.24691358024691357</v>
       </c>
       <c r="L15" s="22">
-        <f>L4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="M15" s="50">
-        <f>M4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.7407407407407407</v>
       </c>
       <c r="N15" s="50">
-        <f>N4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.86419753086419748</v>
       </c>
       <c r="O15" s="22">
-        <f>O4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.16049382716049382</v>
       </c>
       <c r="P15" s="22">
-        <f>P4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.34567901234567899</v>
       </c>
       <c r="Q15" s="50">
-        <f>Q4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.67901234567901236</v>
       </c>
       <c r="R15" s="50">
-        <f>R4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.83950617283950613</v>
       </c>
       <c r="S15" s="27">
-        <f>S4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>4.9382716049382713E-2</v>
       </c>
       <c r="T15" s="27">
-        <f>T4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="U15" s="27">
-        <f>U4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.25925925925925924</v>
       </c>
       <c r="V15" s="54">
-        <f>V4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.49382716049382713</v>
       </c>
       <c r="W15" s="27">
-        <f>W4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="X15" s="27">
-        <f>X4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="Y15" s="27">
-        <f>Y4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="Z15" s="54">
-        <f>Z4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.46913580246913578</v>
       </c>
       <c r="AA15" s="32">
-        <f>AA4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.1728395061728395</v>
       </c>
       <c r="AB15" s="32">
-        <f>AB4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.38271604938271603</v>
       </c>
       <c r="AC15" s="32">
-        <f>AC4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.64197530864197527</v>
       </c>
       <c r="AD15" s="58">
-        <f>AD4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.83950617283950613</v>
       </c>
       <c r="AE15" s="32">
-        <f>AE4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="AF15" s="32">
-        <f>AF4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.24691358024691357</v>
       </c>
       <c r="AG15" s="32">
-        <f>AG4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="AH15" s="58">
-        <f>AH4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.83950617283950613</v>
       </c>
       <c r="AI15" s="37">
-        <f>AI4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.24691358024691357</v>
       </c>
       <c r="AJ15" s="37">
-        <f>AJ4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.53086419753086422</v>
       </c>
       <c r="AK15" s="62">
-        <f>AK4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.75308641975308643</v>
       </c>
       <c r="AL15" s="62">
-        <f>AL4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="AM15" s="37">
-        <f>AM4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.18518518518518517</v>
       </c>
       <c r="AN15" s="37">
-        <f>AN4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.34567901234567899</v>
       </c>
       <c r="AO15" s="62">
-        <f>AO4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.69135802469135799</v>
       </c>
       <c r="AP15" s="62">
-        <f>AP4/$B$1</f>
+        <f t="shared" si="3"/>
         <v>0.86419753086419748</v>
       </c>
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>A5</f>
+        <f t="shared" si="2"/>
         <v>Very unlikely</v>
       </c>
       <c r="B16">
-        <f>B5</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C16" s="17">
-        <f>C5/$B$1</f>
+        <f t="shared" ref="C16:AP16" si="4">C5/$B$1</f>
         <v>0.13580246913580246</v>
       </c>
       <c r="D16" s="17">
-        <f>D5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.32098765432098764</v>
       </c>
       <c r="E16" s="17">
-        <f>E5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.30864197530864196</v>
       </c>
       <c r="F16" s="46">
-        <f>F5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="G16" s="17">
-        <f>G5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H16" s="17">
-        <f>H5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I16" s="17">
-        <f>I5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.29629629629629628</v>
       </c>
       <c r="J16" s="46">
-        <f>J5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="K16" s="22">
-        <f>K5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.1728395061728395</v>
       </c>
       <c r="L16" s="22">
-        <f>L5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.23456790123456789</v>
       </c>
       <c r="M16" s="50">
-        <f>M5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.14814814814814814</v>
       </c>
       <c r="N16" s="50">
-        <f>N5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="O16" s="22">
-        <f>O5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.12345679012345678</v>
       </c>
       <c r="P16" s="22">
-        <f>P5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.1728395061728395</v>
       </c>
       <c r="Q16" s="50">
-        <f>Q5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="R16" s="50">
-        <f>R5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>4.9382716049382713E-2</v>
       </c>
       <c r="S16" s="27">
-        <f>S5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>6.1728395061728392E-2</v>
       </c>
       <c r="T16" s="27">
-        <f>T5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.12345679012345678</v>
       </c>
       <c r="U16" s="27">
-        <f>U5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.24691358024691357</v>
       </c>
       <c r="V16" s="54">
-        <f>V5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.25925925925925924</v>
       </c>
       <c r="W16" s="27">
-        <f>W5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>6.1728395061728392E-2</v>
       </c>
       <c r="X16" s="27">
-        <f>X5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="Y16" s="27">
-        <f>Y5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="Z16" s="54">
-        <f>Z5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.19753086419753085</v>
       </c>
       <c r="AA16" s="32">
-        <f>AA5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.18518518518518517</v>
       </c>
       <c r="AB16" s="32">
-        <f>AB5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.25925925925925924</v>
       </c>
       <c r="AC16" s="32">
-        <f>AC5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.19753086419753085</v>
       </c>
       <c r="AD16" s="58">
-        <f>AD5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>6.1728395061728392E-2</v>
       </c>
       <c r="AE16" s="32">
-        <f>AE5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>9.8765432098765427E-2</v>
       </c>
       <c r="AF16" s="32">
-        <f>AF5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.19753086419753085</v>
       </c>
       <c r="AG16" s="32">
-        <f>AG5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.14814814814814814</v>
       </c>
       <c r="AH16" s="58">
-        <f>AH5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>6.1728395061728392E-2</v>
       </c>
       <c r="AI16" s="37">
-        <f>AI5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.16049382716049382</v>
       </c>
       <c r="AJ16" s="37">
-        <f>AJ5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.13580246913580246</v>
       </c>
       <c r="AK16" s="62">
-        <f>AK5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.16049382716049382</v>
       </c>
       <c r="AL16" s="62">
-        <f>AL5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="AM16" s="37">
-        <f>AM5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="AN16" s="37">
-        <f>AN5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.20987654320987653</v>
       </c>
       <c r="AO16" s="62">
-        <f>AO5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>0.20987654320987653</v>
       </c>
       <c r="AP16" s="62">
-        <f>AP5/$B$1</f>
+        <f t="shared" si="4"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>A6</f>
+        <f t="shared" si="2"/>
         <v>Somewhat unlikely</v>
       </c>
       <c r="B17">
-        <f>B6</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C17" s="17">
-        <f>C6/$B$1</f>
+        <f t="shared" ref="C17:AP17" si="5">C6/$B$1</f>
         <v>0.24691358024691357</v>
       </c>
       <c r="D17" s="17">
-        <f>D6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.18518518518518517</v>
       </c>
       <c r="E17" s="17">
-        <f>E6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="F17" s="46">
-        <f>F6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="G17" s="17">
-        <f>G6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>4.9382716049382713E-2</v>
       </c>
       <c r="H17" s="17">
-        <f>H6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>9.8765432098765427E-2</v>
       </c>
       <c r="I17" s="17">
-        <f>I6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="J17" s="46">
-        <f>J6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.12345679012345678</v>
       </c>
       <c r="K17" s="22">
-        <f>K6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.16049382716049382</v>
       </c>
       <c r="L17" s="22">
-        <f>L6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.16049382716049382</v>
       </c>
       <c r="M17" s="50">
-        <f>M6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>4.9382716049382713E-2</v>
       </c>
       <c r="N17" s="50">
-        <f>N6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>6.1728395061728392E-2</v>
       </c>
       <c r="O17" s="22">
-        <f>O6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.16049382716049382</v>
       </c>
       <c r="P17" s="22">
-        <f>P6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.24691358024691357</v>
       </c>
       <c r="Q17" s="50">
-        <f>Q6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="R17" s="50">
-        <f>R6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="S17" s="27">
-        <f>S6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.12345679012345678</v>
       </c>
       <c r="T17" s="27">
-        <f>T6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.19753086419753085</v>
       </c>
       <c r="U17" s="27">
-        <f>U6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.29629629629629628</v>
       </c>
       <c r="V17" s="54">
-        <f>V6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="W17" s="27">
-        <f>W6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>4.9382716049382713E-2</v>
       </c>
       <c r="X17" s="27">
-        <f>X6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.13580246913580246</v>
       </c>
       <c r="Y17" s="27">
-        <f>Y6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.23456790123456789</v>
       </c>
       <c r="Z17" s="54">
-        <f>Z6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.14814814814814814</v>
       </c>
       <c r="AA17" s="32">
-        <f>AA6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.16049382716049382</v>
       </c>
       <c r="AB17" s="32">
-        <f>AB6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.19753086419753085</v>
       </c>
       <c r="AC17" s="32">
-        <f>AC6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>8.6419753086419748E-2</v>
       </c>
       <c r="AD17" s="58">
-        <f>AD6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="AE17" s="32">
-        <f>AE6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.18518518518518517</v>
       </c>
       <c r="AF17" s="32">
-        <f>AF6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="AG17" s="32">
-        <f>AG6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.12345679012345678</v>
       </c>
       <c r="AH17" s="58">
-        <f>AH6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>4.9382716049382713E-2</v>
       </c>
       <c r="AI17" s="37">
-        <f>AI6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.14814814814814814</v>
       </c>
       <c r="AJ17" s="37">
-        <f>AJ6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.19753086419753085</v>
       </c>
       <c r="AK17" s="62">
-        <f>AK6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="AL17" s="62">
-        <f>AL6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="AM17" s="37">
-        <f>AM6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="AN17" s="37">
-        <f>AN6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>0.18518518518518517</v>
       </c>
       <c r="AO17" s="62">
-        <f>AO6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="AP17" s="62">
-        <f>AP6/$B$1</f>
+        <f t="shared" si="5"/>
         <v>2.4691358024691357E-2</v>
       </c>
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <f>A7</f>
+        <f t="shared" si="2"/>
         <v>Somewhat likely</v>
       </c>
       <c r="B18">
-        <f>B7</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C18" s="17">
-        <f>C7/$B$1</f>
+        <f t="shared" ref="C18:AP18" si="6">C7/$B$1</f>
         <v>0.24691358024691357</v>
       </c>
       <c r="D18" s="17">
-        <f>D7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.24691358024691357</v>
       </c>
       <c r="E18" s="17">
-        <f>E7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="F18" s="46">
-        <f>F7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>6.1728395061728392E-2</v>
       </c>
       <c r="G18" s="17">
-        <f>G7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.23456790123456789</v>
       </c>
       <c r="H18" s="17">
-        <f>H7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.39506172839506171</v>
       </c>
       <c r="I18" s="17">
-        <f>I7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.20987654320987653</v>
       </c>
       <c r="J18" s="46">
-        <f>J7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="K18" s="22">
-        <f>K7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.24691358024691357</v>
       </c>
       <c r="L18" s="22">
-        <f>L7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="M18" s="50">
-        <f>M7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="N18" s="50">
-        <f>N7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="O18" s="22">
-        <f>O7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.19753086419753085</v>
       </c>
       <c r="P18" s="22">
-        <f>P7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.14814814814814814</v>
       </c>
       <c r="Q18" s="50">
-        <f>Q7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R18" s="50">
-        <f>R7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>4.9382716049382713E-2</v>
       </c>
       <c r="S18" s="27">
-        <f>S7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="T18" s="27">
-        <f>T7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.43209876543209874</v>
       </c>
       <c r="U18" s="27">
-        <f>U7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.14814814814814814</v>
       </c>
       <c r="V18" s="54">
-        <f>V7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>4.9382716049382713E-2</v>
       </c>
       <c r="W18" s="27">
-        <f>W7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.16049382716049382</v>
       </c>
       <c r="X18" s="27">
-        <f>X7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.27160493827160492</v>
       </c>
       <c r="Y18" s="27">
-        <f>Y7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="Z18" s="54">
-        <f>Z7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.12345679012345678</v>
       </c>
       <c r="AA18" s="32">
-        <f>AA7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.29629629629629628</v>
       </c>
       <c r="AB18" s="32">
-        <f>AB7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.13580246913580246</v>
       </c>
       <c r="AC18" s="32">
-        <f>AC7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="AD18" s="58">
-        <f>AD7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="AE18" s="32">
-        <f>AE7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.18518518518518517</v>
       </c>
       <c r="AF18" s="32">
-        <f>AF7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.1728395061728395</v>
       </c>
       <c r="AG18" s="32">
-        <f>AG7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>4.9382716049382713E-2</v>
       </c>
       <c r="AH18" s="58">
-        <f>AH7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="AI18" s="37">
-        <f>AI7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.27160493827160492</v>
       </c>
       <c r="AJ18" s="37">
-        <f>AJ7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="AK18" s="62">
-        <f>AK7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="AL18" s="62">
-        <f>AL7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>4.9382716049382713E-2</v>
       </c>
       <c r="AM18" s="37">
-        <f>AM7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="AN18" s="37">
-        <f>AN7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>0.18518518518518517</v>
       </c>
       <c r="AO18" s="62">
-        <f>AO7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="AP18" s="62">
-        <f>AP7/$B$1</f>
+        <f t="shared" si="6"/>
         <v>7.407407407407407E-2</v>
       </c>
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <f>A8</f>
+        <f t="shared" si="2"/>
         <v>Very likely</v>
       </c>
       <c r="B19">
-        <f>B8</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C19" s="17">
-        <f>C8/$B$1</f>
+        <f t="shared" ref="C19:AP19" si="7">C8/$B$1</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="D19" s="17">
-        <f>D8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.13580246913580246</v>
       </c>
       <c r="E19" s="17">
-        <f>E8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="F19" s="46">
-        <f>F8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="G19" s="17">
-        <f>G8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.34567901234567899</v>
       </c>
       <c r="H19" s="17">
-        <f>H8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.2839506172839506</v>
       </c>
       <c r="I19" s="17">
-        <f>I8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="J19" s="46">
-        <f>J8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="K19" s="22">
-        <f>K8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.13580246913580246</v>
       </c>
       <c r="L19" s="22">
-        <f>L8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>4.9382716049382713E-2</v>
       </c>
       <c r="M19" s="50">
-        <f>M8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N19" s="50">
-        <f>N8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="O19" s="22">
-        <f>O8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.1728395061728395</v>
       </c>
       <c r="P19" s="22">
-        <f>P8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>8.6419753086419748E-2</v>
       </c>
       <c r="Q19" s="50">
-        <f>Q8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="R19" s="50">
-        <f>R8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="S19" s="27">
-        <f>S8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.25925925925925924</v>
       </c>
       <c r="T19" s="27">
-        <f>T8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.16049382716049382</v>
       </c>
       <c r="U19" s="27">
-        <f>U8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="V19" s="54">
-        <f>V8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="W19" s="27">
-        <f>W8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.2839506172839506</v>
       </c>
       <c r="X19" s="27">
-        <f>X8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.37037037037037035</v>
       </c>
       <c r="Y19" s="27">
-        <f>Y8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="Z19" s="54">
-        <f>Z8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="AA19" s="32">
-        <f>AA8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="AB19" s="32">
-        <f>AB8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="AC19" s="32">
-        <f>AC8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="AD19" s="58">
-        <f>AD8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="AE19" s="32">
-        <f>AE8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.20987654320987653</v>
       </c>
       <c r="AF19" s="32">
-        <f>AF8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.13580246913580246</v>
       </c>
       <c r="AG19" s="32">
-        <f>AG8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="AH19" s="58">
-        <f>AH8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="AI19" s="37">
-        <f>AI8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>8.6419753086419748E-2</v>
       </c>
       <c r="AJ19" s="37">
-        <f>AJ8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="AK19" s="62">
-        <f>AK8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="AL19" s="62">
-        <f>AL8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="AM19" s="37">
-        <f>AM8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="AN19" s="37">
-        <f>AN8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>4.9382716049382713E-2</v>
       </c>
       <c r="AO19" s="62">
-        <f>AO8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="AP19" s="62">
-        <f>AP8/$B$1</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <f>A9</f>
+        <f t="shared" si="2"/>
         <v>Absolutely</v>
       </c>
       <c r="B20">
-        <f>B9</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C20" s="17">
-        <f>C9/$B$1</f>
+        <f t="shared" ref="C20:AP20" si="8">C9/$B$1</f>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="D20" s="17">
-        <f>D9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E20" s="17">
-        <f>E9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F20" s="46">
-        <f>F9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="G20" s="17">
-        <f>G9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0.34567901234567899</v>
       </c>
       <c r="H20" s="17">
-        <f>H9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0.12345679012345678</v>
       </c>
       <c r="I20" s="17">
-        <f>I9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="J20" s="46">
-        <f>J9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="K20" s="22">
-        <f>K9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="L20" s="22">
-        <f>L9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M20" s="50">
-        <f>M9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="N20" s="50">
-        <f>N9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="O20" s="22">
-        <f>O9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0.18518518518518517</v>
       </c>
       <c r="P20" s="22">
-        <f>P9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q20" s="50">
-        <f>Q9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="R20" s="50">
-        <f>R9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="S20" s="27">
-        <f>S9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0.1728395061728395</v>
       </c>
       <c r="T20" s="27">
-        <f>T9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="U20" s="27">
-        <f>U9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="V20" s="54">
-        <f>V9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>6.1728395061728392E-2</v>
       </c>
       <c r="W20" s="27">
-        <f>W9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0.41975308641975306</v>
       </c>
       <c r="X20" s="27">
-        <f>X9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0.12345679012345678</v>
       </c>
       <c r="Y20" s="27">
-        <f>Y9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="Z20" s="54">
-        <f>Z9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="AA20" s="32">
-        <f>AA9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="AB20" s="32">
-        <f>AB9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC20" s="32">
-        <f>AC9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="AD20" s="58">
-        <f>AD9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="AE20" s="32">
-        <f>AE9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0.20987654320987653</v>
       </c>
       <c r="AF20" s="32">
-        <f>AF9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="AG20" s="32">
-        <f>AG9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH20" s="58">
-        <f>AH9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI20" s="37">
-        <f>AI9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>8.6419753086419748E-2</v>
       </c>
       <c r="AJ20" s="37">
-        <f>AJ9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="AK20" s="62">
-        <f>AK9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="AL20" s="62">
-        <f>AL9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AM20" s="37">
-        <f>AM9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0.18518518518518517</v>
       </c>
       <c r="AN20" s="37">
-        <f>AN9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>2.4691358024691357E-2</v>
       </c>
       <c r="AO20" s="62">
-        <f>AO9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>1.2345679012345678E-2</v>
       </c>
       <c r="AP20" s="62">
-        <f>AP9/$B$1</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -17662,159 +17892,159 @@
         <v>1</v>
       </c>
       <c r="D21" s="18">
-        <f t="shared" ref="D21:AP21" si="2">SUM(D15:D20)</f>
+        <f t="shared" ref="D21:AP21" si="9">SUM(D15:D20)</f>
         <v>1</v>
       </c>
       <c r="E21" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="F21" s="47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="G21" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="H21" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="I21" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="J21" s="47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="K21" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="L21" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M21" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="N21" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O21" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="P21" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Q21" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="R21" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="S21" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="T21" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="U21" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="V21" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="W21" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="X21" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Y21" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="Z21" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA21" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="AB21" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="AC21" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AD21" s="59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AE21" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AF21" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="AG21" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AH21" s="59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI21" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AJ21" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="AK21" s="63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="AL21" s="63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AM21" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AN21" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="AO21" s="63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AP21" s="63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -18001,6 +18231,134 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{A7C7356A-04E5-AC42-BF60-A760041C6825}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Risk Questions Distribution'!C4:C9</xm:f>
+              <xm:sqref>C12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{8B743EE6-7F6B-CA43-8F0A-F70AAF8BB3D7}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Risk Questions Distribution'!D4:D9</xm:f>
+              <xm:sqref>D12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{D4C1ED6C-C688-664F-9538-E14694FB0C71}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Risk Questions Distribution'!E4:E9</xm:f>
+              <xm:sqref>E12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{B209398A-7466-6C42-A452-4D9AE870ADCB}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Risk Questions Distribution'!F4:F9</xm:f>
+              <xm:sqref>F12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{334F7EB0-7A0A-E947-AB3C-331E76789729}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Risk Questions Distribution'!G4:G9</xm:f>
+              <xm:sqref>G12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{8E5F7B1C-F041-4849-A03A-3459AC94899B}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Risk Questions Distribution'!H4:H9</xm:f>
+              <xm:sqref>H12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{E822618A-A8B7-C845-8073-6AA4CDD333BE}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Risk Questions Distribution'!I4:I9</xm:f>
+              <xm:sqref>I12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{235DCE6C-3D64-AB42-8ACA-9A3327AAFC6F}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Risk Questions Distribution'!J4:J9</xm:f>
+              <xm:sqref>J12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{2763537E-67CF-7147-AE57-3F18B5239863}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
@@ -18141,141 +18499,13 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{235DCE6C-3D64-AB42-8ACA-9A3327AAFC6F}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Risk Questions Distribution'!J4:J9</xm:f>
-              <xm:sqref>J12</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{E822618A-A8B7-C845-8073-6AA4CDD333BE}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Risk Questions Distribution'!I4:I9</xm:f>
-              <xm:sqref>I12</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{8E5F7B1C-F041-4849-A03A-3459AC94899B}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Risk Questions Distribution'!H4:H9</xm:f>
-              <xm:sqref>H12</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{334F7EB0-7A0A-E947-AB3C-331E76789729}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Risk Questions Distribution'!G4:G9</xm:f>
-              <xm:sqref>G12</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{B209398A-7466-6C42-A452-4D9AE870ADCB}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Risk Questions Distribution'!F4:F9</xm:f>
-              <xm:sqref>F12</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{D4C1ED6C-C688-664F-9538-E14694FB0C71}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Risk Questions Distribution'!E4:E9</xm:f>
-              <xm:sqref>E12</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{8B743EE6-7F6B-CA43-8F0A-F70AAF8BB3D7}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Risk Questions Distribution'!D4:D9</xm:f>
-              <xm:sqref>D12</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{A7C7356A-04E5-AC42-BF60-A760041C6825}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Risk Questions Distribution'!C4:C9</xm:f>
-              <xm:sqref>C12</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
@@ -18292,7 +18522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>

</xml_diff>